<commit_message>
Handle midnight and date change.
Explanation of Changes:
Case 1: Spans from AM to PM

If recordStartTime is in the morning (AM) and currentTime is in the afternoon (PM), split the highlight at 12:00 PM.
Case 2: Spans from PM to AM

If recordStartTime is in the evening (PM) and currentTime is in the early morning (AM), split the highlight at midnight.
Default Case

For time ranges that don't span across either 12:00 PM or midnight, the behavior remains the same as before.
This ensures the time range is correctly represented in all edge cases.
</commit_message>
<xml_diff>
--- a/AnalogClock activity config.xlsx
+++ b/AnalogClock activity config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\AnalogClockTimeManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AACB6D-6508-4580-B0AA-E718A40EA271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD0573D-81A2-4425-A99E-354288AF796E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{4688EFD4-36D5-428E-BEE4-121022B2E5CC}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{4688EFD4-36D5-428E-BEE4-121022B2E5CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Button ID</t>
     <phoneticPr fontId="2"/>
@@ -65,13 +65,6 @@
   </si>
   <si>
     <t>メル・ココ</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>仕事</t>
-    <rPh sb="0" eb="2">
-      <t>シゴト</t>
-    </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -133,6 +126,62 @@
   </si>
   <si>
     <t>Btn_009</t>
+  </si>
+  <si>
+    <t>仕事-段取り</t>
+    <rPh sb="0" eb="2">
+      <t>シゴト</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ダンド</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>仕事-Delegate</t>
+    <rPh sb="0" eb="2">
+      <t>シゴト</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>仕事-Call</t>
+    <rPh sb="0" eb="2">
+      <t>シゴト</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>仕事-作業</t>
+    <rPh sb="0" eb="2">
+      <t>シゴト</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>サギョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>仕事-思考</t>
+    <rPh sb="0" eb="2">
+      <t>シゴト</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>シコウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Btn_010</t>
+  </si>
+  <si>
+    <t>Btn_011</t>
+  </si>
+  <si>
+    <t>Btn_012</t>
+  </si>
+  <si>
+    <t>Btn_013</t>
   </si>
 </sst>
 </file>
@@ -168,7 +217,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,19 +268,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF808080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF663300"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000099"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,7 +323,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -285,6 +358,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -295,6 +380,14 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF000099"/>
+      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFFFFF66"/>
+      <color rgb="FFFFFF00"/>
+      <color rgb="FFCC9900"/>
+      <color rgb="FF663300"/>
+      <color rgb="FFFFFFCC"/>
       <color rgb="FF808080"/>
       <color rgb="FFD9D9D9"/>
     </mruColors>
@@ -627,13 +720,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57624C22-0333-41EB-A72E-D82F2DE6B244}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -654,16 +747,16 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -672,7 +765,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -681,57 +774,93 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="C5" s="14"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="10"/>
+        <v>21</v>
+      </c>
+      <c r="C10" s="11"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="13"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Revert "Handle midnight and date change."
This reverts commit 9b263182335d7db8f67292e7af4ee84b5ba0fa5d.
</commit_message>
<xml_diff>
--- a/AnalogClock activity config.xlsx
+++ b/AnalogClock activity config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\AnalogClockTimeManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD0573D-81A2-4425-A99E-354288AF796E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AACB6D-6508-4580-B0AA-E718A40EA271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{4688EFD4-36D5-428E-BEE4-121022B2E5CC}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{4688EFD4-36D5-428E-BEE4-121022B2E5CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Button ID</t>
     <phoneticPr fontId="2"/>
@@ -65,6 +65,13 @@
   </si>
   <si>
     <t>メル・ココ</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>仕事</t>
+    <rPh sb="0" eb="2">
+      <t>シゴト</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -126,62 +133,6 @@
   </si>
   <si>
     <t>Btn_009</t>
-  </si>
-  <si>
-    <t>仕事-段取り</t>
-    <rPh sb="0" eb="2">
-      <t>シゴト</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ダンド</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>仕事-Delegate</t>
-    <rPh sb="0" eb="2">
-      <t>シゴト</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>仕事-Call</t>
-    <rPh sb="0" eb="2">
-      <t>シゴト</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>仕事-作業</t>
-    <rPh sb="0" eb="2">
-      <t>シゴト</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>サギョウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>仕事-思考</t>
-    <rPh sb="0" eb="2">
-      <t>シゴト</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>シコウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Btn_010</t>
-  </si>
-  <si>
-    <t>Btn_011</t>
-  </si>
-  <si>
-    <t>Btn_012</t>
-  </si>
-  <si>
-    <t>Btn_013</t>
   </si>
 </sst>
 </file>
@@ -217,7 +168,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,43 +219,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF808080"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF66"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC9900"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF663300"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000099"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,7 +250,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -358,18 +285,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -380,14 +295,6 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF000099"/>
-      <color rgb="FFFF0000"/>
-      <color rgb="FFFFFF99"/>
-      <color rgb="FFFFFF66"/>
-      <color rgb="FFFFFF00"/>
-      <color rgb="FFCC9900"/>
-      <color rgb="FF663300"/>
-      <color rgb="FFFFFFCC"/>
       <color rgb="FF808080"/>
       <color rgb="FFD9D9D9"/>
     </mruColors>
@@ -720,13 +627,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57624C22-0333-41EB-A72E-D82F2DE6B244}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -747,16 +654,16 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -765,7 +672,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -774,93 +681,57 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="14"/>
+        <v>9</v>
+      </c>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="11"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="12"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="13"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="15"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>